<commit_message>
add language to xml attributes
</commit_message>
<xml_diff>
--- a/data-export/WD_missing_entries.xlsx
+++ b/data-export/WD_missing_entries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/data-export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB83FA5-20A9-464E-999C-C8F6D8B9ED53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF8BD1B-7DDD-1E48-909D-0E845C1125D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2500" windowWidth="26440" windowHeight="14180" xr2:uid="{8CB0D64E-A49F-0443-829C-5C738D755DAD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -84,12 +84,6 @@
     <t>rgya gar gyi mkhan po su ren dra bo d+hi</t>
   </si>
   <si>
-    <t>WA0RK0024</t>
-  </si>
-  <si>
-    <t>{'eft:surendrabodhi'}</t>
-  </si>
-  <si>
     <t>translator</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>zhu chen gyi lots+tsha ba ban de ye shes sde</t>
   </si>
   <si>
-    <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
-  </si>
-  <si>
     <t>D140</t>
   </si>
   <si>
@@ -114,12 +105,6 @@
     <t>rgya gar gyi mkhan po pradz+nyA barma</t>
   </si>
   <si>
-    <t>WA0RK0140</t>
-  </si>
-  <si>
-    <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
-  </si>
-  <si>
     <t>revisor</t>
   </si>
   <si>
@@ -138,9 +123,6 @@
     <t>rgya gar gyi mkhan po su ren+d+ra bo d+hi</t>
   </si>
   <si>
-    <t>WA0RK0212</t>
-  </si>
-  <si>
     <t>D980</t>
   </si>
   <si>
@@ -153,9 +135,6 @@
     <t>paN+Di ta su ren+d+ra bo d+hi</t>
   </si>
   <si>
-    <t>WA0RK0312</t>
-  </si>
-  <si>
     <t>zhu chen gyi lo ts+tsha ba ban+de ye shes sde</t>
   </si>
   <si>
@@ -169,12 +148,6 @@
   </si>
   <si>
     <t>rgya gar gyi mkhan po dzi na mi tra</t>
-  </si>
-  <si>
-    <t>WA0RK0313</t>
-  </si>
-  <si>
-    <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
   </si>
   <si>
     <t>P3214</t>
@@ -562,7 +535,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L16"/>
+      <selection activeCell="K2" sqref="K2:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,12 +592,6 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -635,124 +602,94 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -761,46 +698,34 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -809,46 +734,34 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -857,106 +770,79 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>